<commit_message>
Implémentation du niveau 1
Mise en place des règles dans excel et génération des setters et getters
</commit_message>
<xml_diff>
--- a/src/main/resources/ch/hug/service/drools/Rules.xlsx
+++ b/src/main/resources/ch/hug/service/drools/Rules.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\drools-test\src\main\resources\ch\hug\service\drools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse\workspace\drools-test\src\main\resources\ch\hug\service\drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F82745C-6F19-4314-B277-A399C01DA4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25770" windowHeight="8085"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>RuleSet</t>
   </si>
@@ -48,13 +49,97 @@
   </si>
   <si>
     <t>ch.hug.service.drools.DiscountRequest</t>
+  </si>
+  <si>
+    <t>RuleTable Discount</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>CONDITION</t>
+  </si>
+  <si>
+    <t>ACTION</t>
+  </si>
+  <si>
+    <t>$request:DiscountRequest</t>
+  </si>
+  <si>
+    <t>$request.getAge() &lt; $param</t>
+  </si>
+  <si>
+    <t>$request.getAge() &gt; $param</t>
+  </si>
+  <si>
+    <t>$request.getClientType() == $param</t>
+  </si>
+  <si>
+    <t>$request.getAmount()  &gt; ($param)</t>
+  </si>
+  <si>
+    <t>$request.setDiscountValue($param);</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Client VIP</t>
+  </si>
+  <si>
+    <t>Montant</t>
+  </si>
+  <si>
+    <t>REDUCTION</t>
+  </si>
+  <si>
+    <t>NORMAL &lt; 65a &gt; 500m</t>
+  </si>
+  <si>
+    <t>"NORMAL"</t>
+  </si>
+  <si>
+    <t>NORMAL &lt; 65a &gt;2000m</t>
+  </si>
+  <si>
+    <t>NORMAL &lt; 65a &gt; 5000m</t>
+  </si>
+  <si>
+    <t>VIP &lt; 65a &gt; 500m</t>
+  </si>
+  <si>
+    <t>"VIP"</t>
+  </si>
+  <si>
+    <t>VIP &lt; 65a &gt;2000m</t>
+  </si>
+  <si>
+    <t>VIP &lt; 65a &gt; 5000m</t>
+  </si>
+  <si>
+    <t>NORMAL &gt; 65a &gt; 500m</t>
+  </si>
+  <si>
+    <t>NORMAL &gt; 65a &gt;2000m</t>
+  </si>
+  <si>
+    <t>NORMAL &gt; 65a &gt; 5000m</t>
+  </si>
+  <si>
+    <t>VIP &gt; 65a &gt; 500m</t>
+  </si>
+  <si>
+    <t>VIP &gt; 65a &gt;2000m</t>
+  </si>
+  <si>
+    <t>VIP &gt; 65a &gt; 5000m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +152,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,9 +182,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,25 +471,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" customWidth="1"/>
-    <col min="3" max="3" width="82.7109375" customWidth="1"/>
-    <col min="4" max="4" width="75.5703125" customWidth="1"/>
-    <col min="5" max="5" width="38.140625" customWidth="1"/>
-    <col min="6" max="6" width="59.28515625" customWidth="1"/>
-    <col min="7" max="7" width="58.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" customWidth="1"/>
+    <col min="2" max="2" width="38.1796875" customWidth="1"/>
+    <col min="3" max="3" width="82.7265625" customWidth="1"/>
+    <col min="4" max="4" width="75.54296875" customWidth="1"/>
+    <col min="5" max="5" width="38.1796875" customWidth="1"/>
+    <col min="6" max="6" width="58.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -400,7 +499,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -411,7 +510,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="68.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -422,7 +521,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -433,71 +532,308 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8"/>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1">
+        <v>65</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="1">
+        <v>500</v>
+      </c>
+      <c r="F10" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1">
+        <v>65</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F11" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1">
+        <v>65</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F12" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1">
+        <v>65</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="1">
+        <v>500</v>
+      </c>
+      <c r="F13" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1">
+        <v>65</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F14" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1">
+        <v>65</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F15" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1">
+        <v>65</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="1">
+        <v>500</v>
+      </c>
+      <c r="F16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="1">
+        <v>65</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F17" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1">
+        <v>65</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F18" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="1">
+        <v>65</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="1">
+        <v>500</v>
+      </c>
+      <c r="F19" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="1">
+        <v>65</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F20" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="1">
+        <v>65</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F21" s="1">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B7:E7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>